<commit_message>
thêm đơn hàng trực tiếp vào kpi
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_General.xlsx
+++ b/DMS/Templates/Kpi_General.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2439EF3D-09F0-4C73-94D1-77E55D813428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A332D-E5F2-48AC-BB72-C7853852EF12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Tháng 1</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>Vui lòng insert các chỉ tiêu vào theo từng nhân viên</t>
+  </si>
+  <si>
+    <t>SKU/ Đơn hàng trực tiếp</t>
+  </si>
+  <si>
+    <t>Doanh thu đơn hàng trực tiếp</t>
+  </si>
+  <si>
+    <t>Tổng sản lượng đơn hàng trực tiếp</t>
+  </si>
+  <si>
+    <t>Số đơn hàng trực tiếp</t>
   </si>
 </sst>
 </file>
@@ -577,10 +589,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -919,11 +931,123 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+    </row>
+    <row r="15" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -950,9 +1074,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>'Chi tieu'!$A$2:$A$8</xm:f>
+            <xm:f>'Chi tieu'!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C13</xm:sqref>
+          <xm:sqref>C7:C17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -962,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,25 +1103,59 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>